<commit_message>
Updating to new libraries and removing mPDF
</commit_message>
<xml_diff>
--- a/libraries/tbs/plugins/demo/demo_ms_excel.xlsx
+++ b/libraries/tbs/plugins/demo/demo_ms_excel.xlsx
@@ -7,13 +7,15 @@
     <workbookView xWindow="240" yWindow="45" windowWidth="17400" windowHeight="11955"/>
   </bookViews>
   <sheets>
-    <sheet name="Examples part 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Examples part 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Display me" sheetId="4" state="hidden" r:id="rId3"/>
-    <sheet name="Delete me" sheetId="3" r:id="rId4"/>
+    <sheet name="Cells and rows" sheetId="1" r:id="rId1"/>
+    <sheet name="Dynamic columns" sheetId="2" r:id="rId2"/>
+    <sheet name="Charts" sheetId="6" r:id="rId3"/>
+    <sheet name="Pictures" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet to show" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="Sheet to delete" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="the_named_cell">'Delete me'!$B$6</definedName>
+    <definedName name="the_named_cell">'Sheet to delete'!$B$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -81,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>PHP version : [onshow..cst.PHP_VERSION]</t>
   </si>
@@ -181,12 +183,6 @@
   </si>
   <si>
     <t>First Name:</t>
-  </si>
-  <si>
-    <t>[cell1.firstname;block=c]</t>
-  </si>
-  <si>
-    <t>[b2.firstname;block=row]</t>
   </si>
   <si>
     <t>[b2.name]</t>
@@ -271,15 +267,9 @@
     <t>the description (or title) of the picture item, and use</t>
   </si>
   <si>
-    <t>[b2.email_[cell2.val;block=tbs:cell]]</t>
-  </si>
-  <si>
     <t>[a.firstname;block=tbs:row]</t>
   </si>
   <si>
-    <t>Email [cell1.val;block=tbs:cell]</t>
-  </si>
-  <si>
     <t>Merging data with rows</t>
   </si>
   <si>
@@ -289,9 +279,6 @@
     <t>Change the type data in a cell</t>
   </si>
   <si>
-    <t>Chart based on dynamic contents</t>
-  </si>
-  <si>
     <t>Dynamic columns</t>
   </si>
   <si>
@@ -301,9 +288,6 @@
     <t>Delete a sheet</t>
   </si>
   <si>
-    <t>[cell2.score;block=tbs:cell;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>tbs:num</t>
   </si>
   <si>
@@ -328,7 +312,64 @@
     <t>And this named cell too.</t>
   </si>
   <si>
-    <t>Score again</t>
+    <t>Visits</t>
+  </si>
+  <si>
+    <t>[a.visits;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>When you merge the linked data (the table) then the chart is updated.</t>
+  </si>
+  <si>
+    <t>Victories</t>
+  </si>
+  <si>
+    <t>And the merged data can push cells placed under.</t>
+  </si>
+  <si>
+    <t>Unfortunately, this solution needs to have a template with TBS fields instead of illustrating data.</t>
+  </si>
+  <si>
+    <t>↕ texts separated with 1 line in the template</t>
+  </si>
+  <si>
+    <t>OpenTBS can also merge data that is embedded within the chart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can convert a chart linked to ranges into an unlinked chart by selecting the </t>
+  </si>
+  <si>
+    <t>The references in the formula of the series are thus converted into literal values.</t>
+  </si>
+  <si>
+    <t>This is easier for building the chart in the template since you can tune the chard design with a sample of data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    series in the chart, then select the formula bar, and press F9.</t>
+  </si>
+  <si>
+    <t>Show or hide a sheet</t>
+  </si>
+  <si>
+    <t>[c1.firstname;block=tbs:cell]</t>
+  </si>
+  <si>
+    <t>[c2.score;block=tbs:cell;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[b2.firstname;block=tbs:row]</t>
+  </si>
+  <si>
+    <t>Email [dc1.val;block=tbs:cell]</t>
+  </si>
+  <si>
+    <t>[b2.email_[dc2.val;block=tbs:cell]]</t>
+  </si>
+  <si>
+    <t>[ch.team;block=tbs:row]</t>
+  </si>
+  <si>
+    <t>[ch.victories;ope=tbs:num]</t>
   </si>
 </sst>
 </file>
@@ -340,7 +381,7 @@
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,6 +469,13 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -492,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -503,12 +551,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -521,6 +563,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,6 +605,29 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+              </a:rPr>
+              <a:t>Chart with linked data</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -570,30 +642,35 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Score of the team</c:v>
+            <c:strRef>
+              <c:f>Charts!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Victories</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Examples part 1'!$C$20:$C$24</c:f>
+              <c:f>Charts!$H$4:$H$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>[a.name]</c:v>
+                  <c:v>[ch.team;block=tbs:row]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Examples part 1'!$E$20:$E$23</c:f>
+              <c:f>Charts!$I$4:$I$8</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="#,##0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -609,11 +686,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="81547648"/>
-        <c:axId val="81549184"/>
+        <c:axId val="150029056"/>
+        <c:axId val="150030592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81547648"/>
+        <c:axId val="150029056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,7 +699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81549184"/>
+        <c:crossAx val="150030592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -630,7 +707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81549184"/>
+        <c:axId val="150030592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,16 +718,164 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81547648"/>
+        <c:crossAx val="150029056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14519923951661151"/>
+          <c:y val="3.9473684210526314E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Chart with unliked embedded data</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>Newbies</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Padawan</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Regular</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Master</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>26</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>45</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>7</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="150050688"/>
+        <c:axId val="150052224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="150050688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150052224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="150052224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150050688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -667,21 +892,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -695,6 +922,86 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2" descr="The title of the chart is used to merged data from the PHP side." title="chart_members_by_category"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676276</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connecteur droit avec flèche 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4752975" y="590550"/>
+          <a:ext cx="685801" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -704,18 +1011,18 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>663833</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>140044</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="[onshow.x_picture;ope=changepic;tagpos=inside;adjust=inside]"/>
+        <xdr:cNvPr id="2" name="Image 1" descr="[onshow.x_picture;ope=changepic;tagpos=inside;adjust=inside;unique]"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -734,7 +1041,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5543550" y="2847975"/>
+          <a:off x="5543550" y="2857500"/>
           <a:ext cx="1130558" cy="1511644"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1034,7 +1341,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H36"/>
+  <dimension ref="B2:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1103,25 +1410,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="13"/>
-      <c r="E18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="15">
+    <row r="17" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="11"/>
+      <c r="E18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="13">
         <f>SUM(F20:F2005)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -1135,12 +1439,12 @@
         <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
@@ -1149,54 +1453,54 @@
         <v>10</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="13"/>
-      <c r="D21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="15">
-        <f ca="1">SUM( E20         : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="11"/>
+      <c r="D21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="13">
+        <f ca="1">SUM( E20              : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>19</v>
       </c>
@@ -1217,10 +1521,10 @@
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -1228,10 +1532,10 @@
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -1239,18 +1543,17 @@
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1267,23 +1570,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
-        <v>47</v>
+      <c r="B2" s="15" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1293,68 +1596,195 @@
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>42</v>
+      <c r="D8" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>40</v>
+        <v>26</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="s">
-        <v>48</v>
-      </c>
+      <c r="B16" s="15"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="15"/>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="H20" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H21" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H24" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H25" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="4" max="6" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B3"/>
+  <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>33</v>
+    <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1362,7 +1792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B6"/>
   <sheetViews>
@@ -1371,18 +1801,18 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
-        <v>49</v>
+      <c r="B2" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>